<commit_message>
Routine update on 24 June 2020
</commit_message>
<xml_diff>
--- a/求職紀錄.xlsx
+++ b/求職紀錄.xlsx
@@ -10,11 +10,11 @@
   <definedNames>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">data_blockchain!$A$2:$L$121</definedName>
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'資料入數表'!$A$1:$E$19</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_7283CC1A_050D_4148_BC8C_A1DC45B3EB8E_.wvu.FilterData">'資料入數表'!$A$1:$A$85</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_BEBF22FC_9368_438C_9E0A_B25A2A42C26D_.wvu.FilterData">'資料入數表'!$A$1:$A$85</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{7283CC1A-050D-4148-BC8C-A1DC45B3EB8E}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{BEBF22FC-9368-438C-9E0A-B25A2A42C26D}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -4926,7 +4926,7 @@
       </c>
       <c r="L17" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -4956,16 +4956,20 @@
       </c>
       <c r="H18" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I18" s="62"/>
       <c r="J18" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K18" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>14 42900 Game Story Designer
+Mostcore Limited 最核心
+$8500 / Month
+0900 - 1800
+ 大材小用 -- Overqualified ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L18" s="63" t="str">
         <f t="shared" si="3"/>
@@ -5149,7 +5153,7 @@
       </c>
       <c r="L22" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Wr3lMoa5sKex0r+gT68PpD8UO4FmkPscjYWWqPXISK4=</v>
+        <v>Loading...</v>
       </c>
       <c r="M22" s="64"/>
       <c r="N22" s="64"/>
@@ -5179,24 +5183,20 @@
       </c>
       <c r="H23" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Wr3lMoa5sKex0r+gT68PpD8UO4FmkPscjYWWqPXISK4=</v>
+        <v>Loading...</v>
       </c>
       <c r="K23" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>19 42997 全職補習導師
-己思補習學校
-$10000 - $12000 / Month
-1pm-8:30pm 10am-3pm
- 沒有回應 -- No Respond Wr3lMoa5sKex0r+gT68PpD8UO4FmkPscjYWWqPXISK4=</v>
+        <v>Loading...</v>
       </c>
       <c r="L23" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>6QTBMay8tqUwKMz+CmreCbzNR9FIKPr7B+kX1+NkueA=</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -5231,7 +5231,7 @@
       <c r="I24" s="62"/>
       <c r="J24" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>6QTBMay8tqUwKMz+CmreCbzNR9FIKPr7B+kX1+NkueA=</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K24" s="62" t="str">
         <f t="shared" si="2"/>
@@ -5239,11 +5239,11 @@
 香港電台--電視及機構業務部字幕及節目宣傳組
 $10985 - 14125
 0900 - 1800
- 有出席面試機會 -- Interview Attended 6QTBMay8tqUwKMz+CmreCbzNR9FIKPr7B+kX1+NkueA=</v>
+ 有出席面試機會 -- Interview Attended ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L24" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>vTkPYEqXp+ayovkk/0v7V/PPI61/7VvsP/TXPbxNnMU=</v>
+        <v>D2IVwEJge8seFy2qFNnBHMRy7mYL9heFjasAjpfN9EM=</v>
       </c>
       <c r="M24" s="64"/>
       <c r="N24" s="64"/>
@@ -5278,7 +5278,7 @@
       <c r="I25" s="53"/>
       <c r="J25" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>vTkPYEqXp+ayovkk/0v7V/PPI61/7VvsP/TXPbxNnMU=</v>
+        <v>D2IVwEJge8seFy2qFNnBHMRy7mYL9heFjasAjpfN9EM=</v>
       </c>
       <c r="K25" s="53" t="str">
         <f t="shared" si="2"/>
@@ -5286,11 +5286,11 @@
 香港電台 -- 電台部中文台與行政及發展
 $75 / Hours
 0900 - 1800
- 有出席面試機會 -- Interview Attended vTkPYEqXp+ayovkk/0v7V/PPI61/7VvsP/TXPbxNnMU=</v>
+ 有出席面試機會 -- Interview Attended D2IVwEJge8seFy2qFNnBHMRy7mYL9heFjasAjpfN9EM=</v>
       </c>
       <c r="L25" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>a+lwFGKen1iLnmv/47mT5WZQxfFA919DSvgSg0VH+P8=</v>
+        <v>yqI4D3oS5YomOVcm8jj78pIpI38FANaJLqB5rHSgbLU=</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -5325,7 +5325,7 @@
       <c r="I26" s="62"/>
       <c r="J26" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>a+lwFGKen1iLnmv/47mT5WZQxfFA919DSvgSg0VH+P8=</v>
+        <v>yqI4D3oS5YomOVcm8jj78pIpI38FANaJLqB5rHSgbLU=</v>
       </c>
       <c r="K26" s="62" t="str">
         <f t="shared" si="2"/>
@@ -5333,11 +5333,11 @@
 志蓮小學
 $7500 / Month
 3:45 - 5:45
- 有出席面試機會 -- Interview Attended a+lwFGKen1iLnmv/47mT5WZQxfFA919DSvgSg0VH+P8=</v>
+ 有出席面試機會 -- Interview Attended yqI4D3oS5YomOVcm8jj78pIpI38FANaJLqB5rHSgbLU=</v>
       </c>
       <c r="L26" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>mutnVQ74Im3EIX3UXan+Hwon5+ReWqNTubG91blC5Aw=</v>
+        <v>kuDyc8vwylZSegnTGSxDf5RQQRSUPyxiEpS6nMvHbjk=</v>
       </c>
       <c r="M26" s="64"/>
       <c r="N26" s="64"/>
@@ -5372,7 +5372,7 @@
       <c r="I27" s="53"/>
       <c r="J27" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>mutnVQ74Im3EIX3UXan+Hwon5+ReWqNTubG91blC5Aw=</v>
+        <v>kuDyc8vwylZSegnTGSxDf5RQQRSUPyxiEpS6nMvHbjk=</v>
       </c>
       <c r="K27" s="53" t="str">
         <f t="shared" si="2"/>
@@ -5380,7 +5380,7 @@
 中聖教會有限公司
 $65 - 70 /Hours
 3pm-6pm
- 質疑宗教與個人能力之間的關係 -- Religion Related mutnVQ74Im3EIX3UXan+Hwon5+ReWqNTubG91blC5Aw=</v>
+ 質疑宗教與個人能力之間的關係 -- Religion Related kuDyc8vwylZSegnTGSxDf5RQQRSUPyxiEpS6nMvHbjk=</v>
       </c>
       <c r="L27" s="55" t="str">
         <f t="shared" si="3"/>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="L30" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M30" s="64"/>
       <c r="N30" s="64"/>
@@ -5547,16 +5547,20 @@
       </c>
       <c r="H31" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I31" s="53"/>
       <c r="J31" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K31" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>27 43160 Teaching Assistant
+龍翔官立中學
+$15545 / Month
+No state work hours
+ 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L31" s="55" t="str">
         <f t="shared" si="3"/>
@@ -6100,7 +6104,7 @@
       </c>
       <c r="L43" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -6130,20 +6134,23 @@
       </c>
       <c r="H44" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I44" s="62"/>
       <c r="J44" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K44" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>40 43422 初創行政見習生--遊戲開發員
+香港青年協會
+$11000 / Month
+0900 - 1800 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L44" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M44" s="64"/>
       <c r="N44" s="64"/>
@@ -6173,24 +6180,20 @@
       </c>
       <c r="H45" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I45" s="53"/>
       <c r="J45" s="53" t="str">
         <f t="shared" si="5"/>
+        <v>Loading...</v>
+      </c>
+      <c r="K45" s="53" t="str">
+        <f t="shared" si="2"/>
+        <v>Loading...</v>
+      </c>
+      <c r="L45" s="55" t="str">
+        <f t="shared" si="3"/>
         <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="K45" s="53" t="str">
-        <f t="shared" si="2"/>
-        <v>41 43422 Game Designer
-XIAO MA KE JI
-HK 13000 / Month
-0900 - 1800 Sha Tin
- 已婉拒 Refused ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="L45" s="55" t="str">
-        <f t="shared" si="3"/>
-        <v>Loading...</v>
       </c>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -6220,16 +6223,20 @@
       </c>
       <c r="H46" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I46" s="62"/>
       <c r="J46" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K46" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>42 43427 Game Designer
+Planet J
+$14500 / Month Offer
+Degree / Master Level 
+0900 - 1800 Office Job 有出席面試機會 -- Interview Attended ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L46" s="63" t="str">
         <f t="shared" si="3"/>
@@ -6319,7 +6326,7 @@
       </c>
       <c r="L48" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M48" s="64"/>
       <c r="N48" s="64"/>
@@ -6349,20 +6356,20 @@
       </c>
       <c r="H49" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I49" s="53"/>
       <c r="J49" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K49" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>45 43444 3rd Grad-support @ HKDEA 已出席 -- Partake ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L49" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>v0Ojxe3smz4u8XBGCjYxB/qoz1vPQxcwOtlnTCOyIdM=</v>
       </c>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -6397,18 +6404,18 @@
       <c r="I50" s="62"/>
       <c r="J50" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>v0Ojxe3smz4u8XBGCjYxB/qoz1vPQxcwOtlnTCOyIdM=</v>
       </c>
       <c r="K50" s="62" t="str">
         <f t="shared" si="2"/>
         <v>46 43447 福利工作員
 香港小童群益會
 $13000 / Month
-No state working time 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+No state working time 沒有回應 -- No Respond v0Ojxe3smz4u8XBGCjYxB/qoz1vPQxcwOtlnTCOyIdM=</v>
       </c>
       <c r="L50" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>n4l0i1vpzk118Q+jTv3ix+t3e2QXIHnA9tp8a3p46YM=</v>
+        <v>2xAd6O78r6nQYd47r4Ffz+N0OiCWHtBTP0/Ezt0DGzQ=</v>
       </c>
       <c r="M50" s="64"/>
       <c r="N50" s="64"/>
@@ -6443,17 +6450,17 @@
       <c r="I51" s="53"/>
       <c r="J51" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>n4l0i1vpzk118Q+jTv3ix+t3e2QXIHnA9tp8a3p46YM=</v>
+        <v>2xAd6O78r6nQYd47r4Ffz+N0OiCWHtBTP0/Ezt0DGzQ=</v>
       </c>
       <c r="K51" s="53" t="str">
         <f t="shared" si="2"/>
         <v>47 43448 Phone call in
 IT Position
-Six DegreeLink 已出席 -- Partake n4l0i1vpzk118Q+jTv3ix+t3e2QXIHnA9tp8a3p46YM=</v>
+Six DegreeLink 已出席 -- Partake 2xAd6O78r6nQYd47r4Ffz+N0OiCWHtBTP0/Ezt0DGzQ=</v>
       </c>
       <c r="L51" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>NSfNlAhXzyA6FovJUCKchGv3s8yqA4zq/88JOqkTPYs=</v>
+        <v>Loading...</v>
       </c>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -6483,25 +6490,20 @@
       </c>
       <c r="H52" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I52" s="62"/>
       <c r="J52" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>NSfNlAhXzyA6FovJUCKchGv3s8yqA4zq/88JOqkTPYs=</v>
+        <v>Loading...</v>
       </c>
       <c r="K52" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>48 43451 [Invited]
-Programmer
-BIAO XI Technology Limited
-Missing Salary
-Missing Working Time
- 已婉拒 Refused NSfNlAhXzyA6FovJUCKchGv3s8yqA4zq/88JOqkTPYs=</v>
+        <v>Loading...</v>
       </c>
       <c r="L52" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M52" s="64"/>
       <c r="N52" s="64"/>
@@ -6531,20 +6533,23 @@
       </c>
       <c r="H53" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I53" s="53"/>
       <c r="J53" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K53" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>49 43457 IT Support
+香港小童群益會
+$ 15000 / Month
+0900 - 1730 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L53" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
@@ -6574,22 +6579,20 @@
       </c>
       <c r="H54" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I54" s="62"/>
       <c r="J54" s="62" t="str">
         <f t="shared" si="5"/>
+        <v>Loading...</v>
+      </c>
+      <c r="K54" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>Loading...</v>
+      </c>
+      <c r="L54" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="K54" s="62" t="str">
-        <f t="shared" si="2"/>
-        <v>50 43472 青協 珊姑約見
-旺角青年就業起點
- 已出席 -- Partake ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="L54" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v>BpeFkvOBHYftEOGDNa7RYZc77OBrOnUyuhXb/WYu29g=</v>
       </c>
       <c r="M54" s="64"/>
       <c r="N54" s="64"/>
@@ -6624,16 +6627,16 @@
       <c r="I55" s="53"/>
       <c r="J55" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>BpeFkvOBHYftEOGDNa7RYZc77OBrOnUyuhXb/WYu29g=</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K55" s="53" t="str">
         <f t="shared" si="2"/>
         <v>51 43472 旺角青年就業起點
-網絡安全講座 報名 已出席 -- Partake BpeFkvOBHYftEOGDNa7RYZc77OBrOnUyuhXb/WYu29g=</v>
+網絡安全講座 報名 已出席 -- Partake ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L55" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>0s19giLfp3ecHdwTTLqMm5VqTgYzRW64IrEAVLXF334=</v>
+        <v>0paiOH5R2HLT/Ts7A61I1wHuI1XnFevTGImEu18sQlY=</v>
       </c>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
@@ -6668,16 +6671,16 @@
       <c r="I56" s="62"/>
       <c r="J56" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>0s19giLfp3ecHdwTTLqMm5VqTgYzRW64IrEAVLXF334=</v>
+        <v>0paiOH5R2HLT/Ts7A61I1wHuI1XnFevTGImEu18sQlY=</v>
       </c>
       <c r="K56" s="62" t="str">
         <f t="shared" si="2"/>
         <v>52 43472 旺角青年就業起點
-桌遊導師證書課程報名 已出席 -- Partake 0s19giLfp3ecHdwTTLqMm5VqTgYzRW64IrEAVLXF334=</v>
+桌遊導師證書課程報名 已出席 -- Partake 0paiOH5R2HLT/Ts7A61I1wHuI1XnFevTGImEu18sQlY=</v>
       </c>
       <c r="L56" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>x+qnHuT9xQbHtUND+M4ZKsyN69f0VxgvolWIlKXCUr4=</v>
+        <v>Loading...</v>
       </c>
       <c r="M56" s="64"/>
       <c r="N56" s="64"/>
@@ -6707,20 +6710,16 @@
       </c>
       <c r="H57" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I57" s="53"/>
       <c r="J57" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>x+qnHuT9xQbHtUND+M4ZKsyN69f0VxgvolWIlKXCUr4=</v>
+        <v>Loading...</v>
       </c>
       <c r="K57" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>53 43473 選民登記助理 41554
-西貢民政事務處
-$56.5 / Hour (Additional $3.6 per form; Ceil to $992 )
-0900 - 2300pm (8Hours)
- 有出席面試機會 -- Interview Attended x+qnHuT9xQbHtUND+M4ZKsyN69f0VxgvolWIlKXCUr4=</v>
+        <v>Loading...</v>
       </c>
       <c r="L57" s="55" t="str">
         <f t="shared" si="3"/>
@@ -6853,7 +6852,7 @@
       </c>
       <c r="L60" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M60" s="64"/>
       <c r="N60" s="64"/>
@@ -6883,22 +6882,20 @@
       </c>
       <c r="H61" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I61" s="53"/>
       <c r="J61" s="53" t="str">
         <f t="shared" si="5"/>
+        <v>Loading...</v>
+      </c>
+      <c r="K61" s="53" t="str">
+        <f t="shared" si="2"/>
+        <v>Loading...</v>
+      </c>
+      <c r="L61" s="55" t="str">
+        <f t="shared" si="3"/>
         <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="K61" s="53" t="str">
-        <f t="shared" si="2"/>
-        <v>57 43484 遴選
-葵芳青年就業起點
-網絡安全 課程 通過 Pass ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="L61" s="55" t="str">
-        <f t="shared" si="3"/>
-        <v>Loading...</v>
       </c>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
@@ -6928,16 +6925,17 @@
       </c>
       <c r="H62" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I62" s="62"/>
       <c r="J62" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K62" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>58 43508 甲子園 展翅合辦
+資訊科技助理證書課程 家人拒絕 -- Family Refused ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L62" s="63" t="str">
         <f t="shared" si="3"/>
@@ -7027,7 +7025,7 @@
       </c>
       <c r="L64" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M64" s="64"/>
       <c r="N64" s="64"/>
@@ -7057,20 +7055,22 @@
       </c>
       <c r="H65" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I65" s="53"/>
       <c r="J65" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K65" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>61 43519 葵芳青年就業起點
+中英文辦工室應用及打字比賽
+ 已出席 -- Partake ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L65" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>eRV4ogs/wX+490u9uHIgnj/HdvLn5l0YxFX825JjR6o=</v>
       </c>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
@@ -7105,7 +7105,7 @@
       <c r="I66" s="62"/>
       <c r="J66" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>eRV4ogs/wX+490u9uHIgnj/HdvLn5l0YxFX825JjR6o=</v>
       </c>
       <c r="K66" s="62" t="str">
         <f t="shared" si="2"/>
@@ -7113,11 +7113,11 @@
 童行社
 3pm - 4:30pm
 $ 80 - 150 / Hours
- 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+ 沒有回應 -- No Respond eRV4ogs/wX+490u9uHIgnj/HdvLn5l0YxFX825JjR6o=</v>
       </c>
       <c r="L66" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>vCdr53o2m1hzZ9tuDMdWxYtgOJckciqZTIyEfdei0zg=</v>
+        <v>+ibCyo+vDkpxvlJu3toKLsbGoptWYDAEBrt5zzg7yzg=</v>
       </c>
       <c r="M66" s="64"/>
       <c r="N66" s="64"/>
@@ -7152,7 +7152,7 @@
       <c r="I67" s="53"/>
       <c r="J67" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>vCdr53o2m1hzZ9tuDMdWxYtgOJckciqZTIyEfdei0zg=</v>
+        <v>+ibCyo+vDkpxvlJu3toKLsbGoptWYDAEBrt5zzg7yzg=</v>
       </c>
       <c r="K67" s="53" t="str">
         <f t="shared" si="2"/>
@@ -7160,11 +7160,11 @@
 One Plus one Educational Center
 $50 - 70 / Hours
 4pm - 8pm
- 已婉拒 Refused vCdr53o2m1hzZ9tuDMdWxYtgOJckciqZTIyEfdei0zg=</v>
+ 已婉拒 Refused +ibCyo+vDkpxvlJu3toKLsbGoptWYDAEBrt5zzg7yzg=</v>
       </c>
       <c r="L67" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>VuBGtGWFxV20Q0wUFdFbvPrH/Sws8/WoGh1rAB6OC/4=</v>
+        <v>JoUVSuQ29eq6b9suoD4fyWmsqzzHe7ZQahUIbed7uNM=</v>
       </c>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
@@ -7199,7 +7199,7 @@
       <c r="I68" s="62"/>
       <c r="J68" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>VuBGtGWFxV20Q0wUFdFbvPrH/Sws8/WoGh1rAB6OC/4=</v>
+        <v>JoUVSuQ29eq6b9suoD4fyWmsqzzHe7ZQahUIbed7uNM=</v>
       </c>
       <c r="K68" s="62" t="str">
         <f t="shared" si="2"/>
@@ -7207,11 +7207,11 @@
 Unity Game Developer (Analysis Programmer)
 Anchor Point Limited
 $23000 / Month
-0900 - 1800 有出席面試機會 -- Interview Attended VuBGtGWFxV20Q0wUFdFbvPrH/Sws8/WoGh1rAB6OC/4=</v>
+0900 - 1800 有出席面試機會 -- Interview Attended JoUVSuQ29eq6b9suoD4fyWmsqzzHe7ZQahUIbed7uNM=</v>
       </c>
       <c r="L68" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>wzgkW4Bzb/ks1yexIIeIv53S0pEWiXAtoc/e5c8xgNw=</v>
       </c>
       <c r="M68" s="64"/>
       <c r="N68" s="64"/>
@@ -7241,20 +7241,25 @@
       </c>
       <c r="H69" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I69" s="53"/>
       <c r="J69" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>wzgkW4Bzb/ks1yexIIeIv53S0pEWiXAtoc/e5c8xgNw=</v>
       </c>
       <c r="K69" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>65 43526 Cyberport Jobs Fair
+Unity Game Developer
+ESport International Group
+Not state salary
+Not State working time
+ 有出席面試機會 -- Interview Attended wzgkW4Bzb/ks1yexIIeIv53S0pEWiXAtoc/e5c8xgNw=</v>
       </c>
       <c r="L69" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
@@ -7284,24 +7289,20 @@
       </c>
       <c r="H70" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I70" s="62"/>
       <c r="J70" s="62" t="str">
         <f t="shared" si="5"/>
+        <v>Loading...</v>
+      </c>
+      <c r="K70" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>Loading...</v>
+      </c>
+      <c r="L70" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="K70" s="62" t="str">
-        <f t="shared" si="2"/>
-        <v>66 43526 Cyberport Jobs Fair
-Internship of Developer
-AVA Technology
-Not state working time and salary
- 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="L70" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v>nzAN9nl2sdzsLrr4BMyhiCdcGahNVlbGm3H1eb79cHI=</v>
       </c>
       <c r="M70" s="64"/>
       <c r="N70" s="64"/>
@@ -7336,7 +7337,7 @@
       <c r="I71" s="53"/>
       <c r="J71" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>nzAN9nl2sdzsLrr4BMyhiCdcGahNVlbGm3H1eb79cHI=</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K71" s="53" t="str">
         <f t="shared" si="2"/>
@@ -7345,11 +7346,11 @@
 Gamespace Limited
 $15000 / Month
 0900 - 1800 @Cyberport
- 沒有回應 -- No Respond nzAN9nl2sdzsLrr4BMyhiCdcGahNVlbGm3H1eb79cHI=</v>
+ 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L71" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>zGpJuCwiQnMgnguRuglVca0c5+CXCQECaaEV+mRC/9o=</v>
+        <v>LUf2E0ONkALX9IG1GT3VI+7d4KFsSUmuoxaavEKq7oE=</v>
       </c>
       <c r="M71" s="3"/>
       <c r="N71" s="3"/>
@@ -7384,7 +7385,7 @@
       <c r="I72" s="62"/>
       <c r="J72" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>zGpJuCwiQnMgnguRuglVca0c5+CXCQECaaEV+mRC/9o=</v>
+        <v>LUf2E0ONkALX9IG1GT3VI+7d4KFsSUmuoxaavEKq7oE=</v>
       </c>
       <c r="K72" s="62" t="str">
         <f t="shared" si="2"/>
@@ -7393,11 +7394,11 @@
 Gamespace Limited
 $16500 / Month
 0900 - 1800 @Cyberport
- 沒有回應 -- No Respond zGpJuCwiQnMgnguRuglVca0c5+CXCQECaaEV+mRC/9o=</v>
+ 沒有回應 -- No Respond LUf2E0ONkALX9IG1GT3VI+7d4KFsSUmuoxaavEKq7oE=</v>
       </c>
       <c r="L72" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>OvAL45s03Zr4LrX9sq3VTJdmgx/u3Ml80uLrtK6b1xo=</v>
+        <v>Loading...</v>
       </c>
       <c r="M72" s="64"/>
       <c r="N72" s="64"/>
@@ -7427,20 +7428,16 @@
       </c>
       <c r="H73" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I73" s="53"/>
       <c r="J73" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>OvAL45s03Zr4LrX9sq3VTJdmgx/u3Ml80uLrtK6b1xo=</v>
+        <v>Loading...</v>
       </c>
       <c r="K73" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>69 43531 Teacher / Tutor
-Baptist Oi Kwan Social Service HKE Family Dev Service CTR
-$70 - $140 / Hours,  TKO
-3pm - 6pm
- 有出席面試機會 -- Interview Attended OvAL45s03Zr4LrX9sq3VTJdmgx/u3Ml80uLrtK6b1xo=</v>
+        <v>Loading...</v>
       </c>
       <c r="L73" s="55" t="str">
         <f t="shared" si="3"/>
@@ -7573,7 +7570,7 @@
       </c>
       <c r="L76" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M76" s="64"/>
       <c r="N76" s="64"/>
@@ -7603,24 +7600,20 @@
       </c>
       <c r="H77" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I77" s="53"/>
       <c r="J77" s="53" t="str">
         <f t="shared" si="5"/>
+        <v>Loading...</v>
+      </c>
+      <c r="K77" s="53" t="str">
+        <f t="shared" si="2"/>
+        <v>Loading...</v>
+      </c>
+      <c r="L77" s="55" t="str">
+        <f t="shared" si="3"/>
         <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="K77" s="53" t="str">
-        <f t="shared" si="2"/>
-        <v>73 43537 半職導師
-名賢教育有限公司
-$6000 - 7000
-4pm - 8pm
- 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="L77" s="55" t="str">
-        <f t="shared" si="3"/>
-        <v>I+OcKoK3oiuHUFel1pQ6udVmcX0DTM2sK8iP5jIQnwY=</v>
       </c>
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
@@ -7655,7 +7648,7 @@
       <c r="I78" s="62"/>
       <c r="J78" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>I+OcKoK3oiuHUFel1pQ6udVmcX0DTM2sK8iP5jIQnwY=</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K78" s="62" t="str">
         <f t="shared" si="2"/>
@@ -7663,11 +7656,11 @@
 1+1 Education Lim TKO
 $ 70 / Hour
 3pm - 6pm
- 已婉拒 Refused I+OcKoK3oiuHUFel1pQ6udVmcX0DTM2sK8iP5jIQnwY=</v>
+ 已婉拒 Refused ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L78" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>/WNtJu9hWRSKXYhm/RmHX47uYmhYVt/RnrkIbAjp01I=</v>
+        <v>d9mmTRlcrvmUcj4E/xBM1NN8u3yci8BlrqNg8eXevps=</v>
       </c>
       <c r="M78" s="64"/>
       <c r="N78" s="64"/>
@@ -7702,7 +7695,7 @@
       <c r="I79" s="53"/>
       <c r="J79" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>/WNtJu9hWRSKXYhm/RmHX47uYmhYVt/RnrkIbAjp01I=</v>
+        <v>d9mmTRlcrvmUcj4E/xBM1NN8u3yci8BlrqNg8eXevps=</v>
       </c>
       <c r="K79" s="53" t="str">
         <f t="shared" si="2"/>
@@ -7710,7 +7703,7 @@
 德田補習學校
 $55 - 70 / Hours
 4pm - 8pm
- 有出席面試機會 -- Interview Attended /WNtJu9hWRSKXYhm/RmHX47uYmhYVt/RnrkIbAjp01I=</v>
+ 有出席面試機會 -- Interview Attended d9mmTRlcrvmUcj4E/xBM1NN8u3yci8BlrqNg8eXevps=</v>
       </c>
       <c r="L79" s="55" t="str">
         <f t="shared" si="3"/>
@@ -7757,7 +7750,7 @@
       </c>
       <c r="L80" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M80" s="64"/>
       <c r="N80" s="64"/>
@@ -7787,20 +7780,24 @@
       </c>
       <c r="H81" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I81" s="53"/>
       <c r="J81" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K81" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>77 43541 Maths Tutor
+數研陽光(天晉)補習中心
+$12000 - $15000 / Month
+10 am - 7:45pm
+ 大材小用 -- Overqualified ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L81" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>ke6MhBWnaAWwO+cZ84LPI0M+37P91lUU1i38tMlURdo=</v>
       </c>
       <c r="M81" s="3"/>
       <c r="N81" s="3"/>
@@ -7835,18 +7832,18 @@
       <c r="I82" s="62"/>
       <c r="J82" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>ke6MhBWnaAWwO+cZ84LPI0M+37P91lUU1i38tMlURdo=</v>
       </c>
       <c r="K82" s="62" t="str">
         <f t="shared" si="2"/>
         <v>78 43544 一級技術支援服務主任
 炮台山金文泰中學
 $15186 / Month
-Gov Office Hours 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+Gov Office Hours 沒有回應 -- No Respond ke6MhBWnaAWwO+cZ84LPI0M+37P91lUU1i38tMlURdo=</v>
       </c>
       <c r="L82" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>PzTLVyiAEUGESdCrXchGSWhWcdUQ57iPez/Dyix7V3o=</v>
+        <v>fMb6oedBjcHlsSnt0N9BK3YBhRDTWNGS/NbP2Ttzi1E=</v>
       </c>
       <c r="M82" s="64"/>
       <c r="N82" s="64"/>
@@ -7881,7 +7878,7 @@
       <c r="I83" s="53"/>
       <c r="J83" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>PzTLVyiAEUGESdCrXchGSWhWcdUQ57iPez/Dyix7V3o=</v>
+        <v>fMb6oedBjcHlsSnt0N9BK3YBhRDTWNGS/NbP2Ttzi1E=</v>
       </c>
       <c r="K83" s="53" t="str">
         <f t="shared" si="2"/>
@@ -7889,11 +7886,11 @@
 大學教育資助委員會秘書處
 $13435  / Month
 Gov Office Hours
- 沒有回應 -- No Respond PzTLVyiAEUGESdCrXchGSWhWcdUQ57iPez/Dyix7V3o=</v>
+ 沒有回應 -- No Respond fMb6oedBjcHlsSnt0N9BK3YBhRDTWNGS/NbP2Ttzi1E=</v>
       </c>
       <c r="L83" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>d2hOa9mDB1b8qP5cT169oT3MatKGxIzTtzkhj1H7Q0E=</v>
+        <v>Loading...</v>
       </c>
       <c r="M83" s="3"/>
       <c r="N83" s="3"/>
@@ -7923,24 +7920,20 @@
       </c>
       <c r="H84" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I84" s="62"/>
       <c r="J84" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>d2hOa9mDB1b8qP5cT169oT3MatKGxIzTtzkhj1H7Q0E=</v>
+        <v>Loading...</v>
       </c>
       <c r="K84" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>80 43547 常務助理
-政制及內地事務局--選舉事務處所屬
-$12270 / Month
-0900 - 1800
- 已收到申請 Acknowledgement of Application d2hOa9mDB1b8qP5cT169oT3MatKGxIzTtzkhj1H7Q0E=</v>
+        <v>Loading...</v>
       </c>
       <c r="L84" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M84" s="64"/>
       <c r="N84" s="64"/>
@@ -7970,16 +7963,20 @@
       </c>
       <c r="H85" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I85" s="53"/>
       <c r="J85" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K85" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>81 43548 常務助理
+選舉事務處 政制及內地事務局
+$12270 / Month
+Gov Office Time
+ 有出席面試機會 -- Interview Attended ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L85" s="55" t="str">
         <f t="shared" si="3"/>
@@ -8024,7 +8021,7 @@
       </c>
       <c r="L86" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M86" s="64"/>
       <c r="N86" s="64"/>
@@ -8054,20 +8051,24 @@
       </c>
       <c r="H87" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I87" s="53"/>
       <c r="J87" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K87" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>83 43557 合約文員
+民政事務總處——專責事務組
+$12170/Month
+0900 - 1800
+ 已收到申請 Acknowledgement of Application ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L87" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>O/XFe/ULu856nce4TFFNxSJ8uyH9FwBCFHfzYHaOvF0=</v>
       </c>
       <c r="M87" s="3"/>
       <c r="N87" s="3"/>
@@ -8102,18 +8103,18 @@
       <c r="I88" s="62"/>
       <c r="J88" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>O/XFe/ULu856nce4TFFNxSJ8uyH9FwBCFHfzYHaOvF0=</v>
       </c>
       <c r="K88" s="62" t="str">
         <f t="shared" si="2"/>
         <v>84 43557 合約文員 41565
 專責事務組 民政事務總署
 $12170 / Month
-Gov Office Time 已收到申請 Acknowledgement of Application ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+Gov Office Time 已收到申請 Acknowledgement of Application O/XFe/ULu856nce4TFFNxSJ8uyH9FwBCFHfzYHaOvF0=</v>
       </c>
       <c r="L88" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>wmBy14WOwWcsU3ekE1d+g2wJIOjV4KW+TR8HRUTrYq4=</v>
+        <v>Loading...</v>
       </c>
       <c r="M88" s="64"/>
       <c r="N88" s="64"/>
@@ -8143,20 +8144,16 @@
       </c>
       <c r="H89" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I89" s="53"/>
       <c r="J89" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>wmBy14WOwWcsU3ekE1d+g2wJIOjV4KW+TR8HRUTrYq4=</v>
+        <v>Loading...</v>
       </c>
       <c r="K89" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>85 43567 Data Center Operations Assistant
-HKEAA
-Salary and working time not stated
-Contract up to 31 Aug 2019
- 家人拒絕 -- Family Refused wmBy14WOwWcsU3ekE1d+g2wJIOjV4KW+TR8HRUTrYq4=</v>
+        <v>Loading...</v>
       </c>
       <c r="L89" s="55" t="str">
         <f t="shared" si="3"/>
@@ -8246,7 +8243,7 @@
       </c>
       <c r="L91" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
@@ -8276,20 +8273,23 @@
       </c>
       <c r="H92" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I92" s="62"/>
       <c r="J92" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K92" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>88 43577 Internship of Assessment Technology and Research
+HKEAA
+Salary and working time not stated
+ 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L92" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M92" s="64"/>
       <c r="N92" s="64"/>
@@ -8319,22 +8319,20 @@
       </c>
       <c r="H93" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I93" s="53"/>
       <c r="J93" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="K93" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>89 43577 WorldSkills 2019 Application
-1) Game Level Programming
-2) 3D Modelling and Art 已收到申請 Acknowledgement of Application ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="L93" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>7ZlWBUs3kXmm09lJ+i+xsbCBj/DU8HvVivvJlYYxC+0=</v>
+        <v>Loading...</v>
       </c>
       <c r="M93" s="3"/>
       <c r="N93" s="3"/>
@@ -8364,26 +8362,20 @@
       </c>
       <c r="H94" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I94" s="62"/>
       <c r="J94" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>7ZlWBUs3kXmm09lJ+i+xsbCBj/DU8HvVivvJlYYxC+0=</v>
+        <v>Loading...</v>
       </c>
       <c r="K94" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>90 43577 手機遊戲測試員
-利達網絡有限公司 CR 2593244
-Latersoft
-$500 / Day
-10am - 6pm
-1wk working contract
- 有出席面試機會 -- Interview Attended 7ZlWBUs3kXmm09lJ+i+xsbCBj/DU8HvVivvJlYYxC+0=</v>
+        <v>Loading...</v>
       </c>
       <c r="L94" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>JuDk4cfrpDuMMXqW2KTLbnsyAol89wtoTd4nWim7xiw=</v>
+        <v>Loading...</v>
       </c>
       <c r="M94" s="64"/>
       <c r="N94" s="64"/>
@@ -8413,20 +8405,16 @@
       </c>
       <c r="H95" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I95" s="53"/>
       <c r="J95" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>JuDk4cfrpDuMMXqW2KTLbnsyAol89wtoTd4nWim7xiw=</v>
+        <v>Loading...</v>
       </c>
       <c r="K95" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>91 43578 項目統籌
-觀塘民政事務署--民政事務總署
-$15650 / Month
-Gov Office Time
- 沒有回應 -- No Respond JuDk4cfrpDuMMXqW2KTLbnsyAol89wtoTd4nWim7xiw=</v>
+        <v>Loading...</v>
       </c>
       <c r="L95" s="55" t="str">
         <f t="shared" si="3"/>
@@ -8696,7 +8684,7 @@
       </c>
       <c r="L101" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M101" s="3"/>
       <c r="N101" s="3"/>
@@ -8726,21 +8714,16 @@
       </c>
       <c r="H102" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I102" s="62"/>
       <c r="J102" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="K102" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>98 43583 網頁編輯員
-VAC0113844
-貿易發展局
-$12000 / Month
-Gov Office Time
- 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="L102" s="63" t="str">
         <f t="shared" si="3"/>
@@ -8787,7 +8770,7 @@
       </c>
       <c r="L103" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M103" s="3"/>
       <c r="N103" s="3"/>
@@ -8817,22 +8800,20 @@
       </c>
       <c r="H104" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I104" s="62"/>
       <c r="J104" s="62" t="str">
         <f t="shared" si="5"/>
+        <v>Loading...</v>
+      </c>
+      <c r="K104" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>Loading...</v>
+      </c>
+      <c r="L104" s="63" t="str">
+        <f t="shared" si="3"/>
         <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="K104" s="62" t="str">
-        <f t="shared" si="2"/>
-        <v>100 43589 葵芳青年就業起點
-管理及策略團隊培訓 桌遊活動
-04/05/2019 1130-1830 主辦取消 Cancelled (Org) ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
-      </c>
-      <c r="L104" s="63" t="str">
-        <f t="shared" si="3"/>
-        <v>hXCuqS78DNXQIALXQ1JBcitJJe6T+J+d0ESCDOVO5Rs=</v>
       </c>
       <c r="M104" s="64"/>
       <c r="N104" s="64"/>
@@ -8867,7 +8848,7 @@
       <c r="I105" s="53"/>
       <c r="J105" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>hXCuqS78DNXQIALXQ1JBcitJJe6T+J+d0ESCDOVO5Rs=</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K105" s="53" t="str">
         <f t="shared" si="2"/>
@@ -8877,7 +8858,7 @@
 $13000 - 15000
 0900 - 1800 , 5day work bank hoilday
 OT Pay, No exp reqire
- 主事者縮沙 Returned by interviewer hXCuqS78DNXQIALXQ1JBcitJJe6T+J+d0ESCDOVO5Rs=</v>
+ 主事者縮沙 Returned by interviewer ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L105" s="55" t="str">
         <f t="shared" si="3"/>
@@ -9047,7 +9028,7 @@
       </c>
       <c r="L109" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>oPiJh19JK3mwFwdRhMxqhbR+i2bHiMgDoRUQP2cJhoY=</v>
       </c>
       <c r="M109" s="3"/>
       <c r="N109" s="3"/>
@@ -9077,20 +9058,26 @@
       </c>
       <c r="H110" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I110" s="62"/>
       <c r="J110" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>oPiJh19JK3mwFwdRhMxqhbR+i2bHiMgDoRUQP2cJhoY=</v>
       </c>
       <c r="K110" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>106 43607 資訊科技支援主任
+觀塘官立小學(秀明道)
+$19030
+0845 - 1730
+Gov Office Hour
+Renewable Contact
+ 有出席第二次面試機會 -- 2nd Interview Attended oPiJh19JK3mwFwdRhMxqhbR+i2bHiMgDoRUQP2cJhoY=</v>
       </c>
       <c r="L110" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>iOsncUhl/cgb5qW+j9GiVnRuipp0frIezDcilyxrazo=</v>
       </c>
       <c r="M110" s="64"/>
       <c r="N110" s="64"/>
@@ -9125,7 +9112,7 @@
       <c r="I111" s="53"/>
       <c r="J111" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>iOsncUhl/cgb5qW+j9GiVnRuipp0frIezDcilyxrazo=</v>
       </c>
       <c r="K111" s="53" t="str">
         <f t="shared" si="2"/>
@@ -9134,11 +9121,11 @@
 VAC0114092
 $10400
 0900 - 1800
-Gov Office Time 已婉拒 Refused ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+Gov Office Time 已婉拒 Refused iOsncUhl/cgb5qW+j9GiVnRuipp0frIezDcilyxrazo=</v>
       </c>
       <c r="L111" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>Bv8kKYxifvZBOUIkBK72I3Ko93jvOAh8RfAcTheLRs4=</v>
       </c>
       <c r="M111" s="3"/>
       <c r="N111" s="3"/>
@@ -9168,16 +9155,21 @@
       </c>
       <c r="H112" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I112" s="62"/>
       <c r="J112" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>Bv8kKYxifvZBOUIkBK72I3Ko93jvOAh8RfAcTheLRs4=</v>
       </c>
       <c r="K112" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>108 43608 Photo Retoucher
+Hong Kong Trade Development Council
+VAC0113843
+$12000
+Gov Office Time
+ 沒有回應 -- No Respond Bv8kKYxifvZBOUIkBK72I3Ko93jvOAh8RfAcTheLRs4=</v>
       </c>
       <c r="L112" s="63" t="str">
         <f t="shared" si="3"/>
@@ -9358,7 +9350,7 @@
       </c>
       <c r="L116" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>Loading...</v>
+        <v>zOYr6EFuCyixk6JkVryimxAoquSUjpxxMOWZ9LopKv8=</v>
       </c>
       <c r="M116" s="64"/>
       <c r="N116" s="64"/>
@@ -9388,20 +9380,23 @@
       </c>
       <c r="H117" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>Loading...</v>
+        <v>T</v>
       </c>
       <c r="I117" s="53"/>
       <c r="J117" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>Loading...</v>
+        <v>zOYr6EFuCyixk6JkVryimxAoquSUjpxxMOWZ9LopKv8=</v>
       </c>
       <c r="K117" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>Loading...</v>
+        <v>113 43613 3rd Fresh Graduate Support Scheme
+2019  -- 3rd CEO Master Talk
+Job and Career Talk Show
+ 已出席 -- Partake zOYr6EFuCyixk6JkVryimxAoquSUjpxxMOWZ9LopKv8=</v>
       </c>
       <c r="L117" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="M117" s="3"/>
       <c r="N117" s="3"/>
@@ -9431,21 +9426,20 @@
       </c>
       <c r="H118" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I118" s="62"/>
       <c r="J118" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="K118" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>114 43628 展翅青見計劃 -- 電子教。學支援計劃
-首輪招聘會 病未能出席 ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
+        <v>Loading...</v>
       </c>
       <c r="L118" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>4pj0ziba/F+Q7X38CL90dGMRpbnpfQPvusop55iX/Ws=</v>
+        <v>Loading...</v>
       </c>
       <c r="M118" s="64"/>
       <c r="N118" s="64"/>
@@ -9475,20 +9469,20 @@
       </c>
       <c r="H119" s="53" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I119" s="53"/>
       <c r="J119" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>4pj0ziba/F+Q7X38CL90dGMRpbnpfQPvusop55iX/Ws=</v>
+        <v>Loading...</v>
       </c>
       <c r="K119" s="53" t="str">
         <f t="shared" si="2"/>
-        <v>115 43637 展翅青見計劃 已完成 -- Completed 4pj0ziba/F+Q7X38CL90dGMRpbnpfQPvusop55iX/Ws=</v>
+        <v>Loading...</v>
       </c>
       <c r="L119" s="55" t="str">
         <f t="shared" si="3"/>
-        <v>tpKEFcbLEeIecOpnc7oVsPtacMfJCesEk5vAjoiBnuY=</v>
+        <v>Loading...</v>
       </c>
       <c r="M119" s="3"/>
       <c r="N119" s="3"/>
@@ -9516,24 +9510,20 @@
       </c>
       <c r="H120" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>Loading...</v>
       </c>
       <c r="I120" s="62"/>
       <c r="J120" s="62" t="str">
         <f t="shared" si="5"/>
-        <v>tpKEFcbLEeIecOpnc7oVsPtacMfJCesEk5vAjoiBnuY=</v>
+        <v>Loading...</v>
       </c>
       <c r="K120" s="62" t="str">
         <f t="shared" si="2"/>
-        <v>116 43638 展翅青見 學教支援計劃
-電子教學支援員
-將軍澳官立小學
-08:30 - 17:00  (5, 5.5 day)
-$10,500 聘用 -- Hired tpKEFcbLEeIecOpnc7oVsPtacMfJCesEk5vAjoiBnuY=</v>
+        <v>Loading...</v>
       </c>
       <c r="L120" s="63" t="str">
         <f t="shared" si="3"/>
-        <v>4EqzM/Tf4aO793xxRDf68Gq/0m7/ddoyiTD9wMvYHXg=</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="M120" s="64"/>
       <c r="N120" s="64"/>
@@ -9566,7 +9556,7 @@
       <c r="I121" s="53"/>
       <c r="J121" s="53" t="str">
         <f t="shared" si="5"/>
-        <v>4EqzM/Tf4aO793xxRDf68Gq/0m7/ddoyiTD9wMvYHXg=</v>
+        <v>ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="K121" s="53" t="str">
         <f t="shared" si="2"/>
@@ -9574,7 +9564,7 @@
 電子教學支援員
 順德聯誼總會鄭裕彤中學法團校董會
 07:55 - 17:00  (5, 5.5 day)
-$10,500 - $13,000 沒有回應 -- No Respond 4EqzM/Tf4aO793xxRDf68Gq/0m7/ddoyiTD9wMvYHXg=</v>
+$10,500 - $13,000 沒有回應 -- No Respond ke95Lr1rgcz7Ys9OWvxDjxlu5QQUFW8Z7NGoU/xUY50=</v>
       </c>
       <c r="L121" s="55" t="str">
         <f t="shared" si="3"/>
@@ -11522,7 +11512,7 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{7283CC1A-050D-4148-BC8C-A1DC45B3EB8E}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{BEBF22FC-9368-438C-9E0A-B25A2A42C26D}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$A$85"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>